<commit_message>
Part numbers added to BOM
the .xlsx file
</commit_message>
<xml_diff>
--- a/KiCAD/22257_DevBoard/22257_DevBoard/22257_DevBoard_BOM.xlsx
+++ b/KiCAD/22257_DevBoard/22257_DevBoard/22257_DevBoard_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijd9015\Documents\GitHub\CubeSatTimeCard\KiCAD\22257_DevBoard\22257_DevBoard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijifl\Documents\git\CubeSatTimeCard\KiCAD\22257_DevBoard\22257_DevBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{850F430C-0155-4AB3-894C-0010E45D29CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCE03C6-C294-470D-86D9-BC967EEC3991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{D03156B8-26E2-4495-A144-03235EBE18FC}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="100">
   <si>
     <t>Reference</t>
   </si>
@@ -254,13 +254,79 @@
   </si>
   <si>
     <t>Package_TO_SOT_SMD:SOT-23-5_HandSoldering</t>
+  </si>
+  <si>
+    <t>Digikey Part Number</t>
+  </si>
+  <si>
+    <t>1276-1009-1-ND</t>
+  </si>
+  <si>
+    <t>1276-2087-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1006-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1038-1-ND</t>
+  </si>
+  <si>
+    <t>1276-CL10A476MQ8QRNCCT-ND</t>
+  </si>
+  <si>
+    <t>1276-7076-1-ND</t>
+  </si>
+  <si>
+    <t>350-2037-1-ND</t>
+  </si>
+  <si>
+    <t>277-7450-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> --- </t>
+  </si>
+  <si>
+    <t>ARFX1232-ND</t>
+  </si>
+  <si>
+    <t>P200KDBCT-ND</t>
+  </si>
+  <si>
+    <t>P1.00KHCT-ND</t>
+  </si>
+  <si>
+    <t>P20086CT-ND</t>
+  </si>
+  <si>
+    <t>P20168CT-ND</t>
+  </si>
+  <si>
+    <t>4423-BVT-I-R002-1.0CT-ND</t>
+  </si>
+  <si>
+    <t>296-15819-1-ND</t>
+  </si>
+  <si>
+    <t>296-TPS562202SDRLRCT-ND</t>
+  </si>
+  <si>
+    <t>296-23978-1-ND</t>
+  </si>
+  <si>
+    <t>828-1077-1-ND</t>
+  </si>
+  <si>
+    <t>296-11933-1-ND</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1114,19 +1180,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A680BC4-C5CF-4118-916D-B33298AE80E2}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.75" customWidth="1"/>
-    <col min="2" max="2" width="31.5" customWidth="1"/>
-    <col min="3" max="3" width="8.75" customWidth="1"/>
-    <col min="4" max="4" width="63.125" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" customWidth="1"/>
+    <col min="2" max="4" width="31.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="63.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1134,19 +1202,25 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1154,16 +1228,19 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1171,16 +1248,19 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1188,16 +1268,19 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1205,16 +1288,19 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1222,16 +1308,19 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>9</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1239,16 +1328,19 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1256,16 +1348,19 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>9</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1273,16 +1368,19 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>9</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1290,30 +1388,36 @@
         <v>26</v>
       </c>
       <c r="C10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>27</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" t="s">
         <v>30</v>
       </c>
-      <c r="E11">
+      <c r="G11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1321,16 +1425,19 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>33</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1338,30 +1445,36 @@
         <v>35</v>
       </c>
       <c r="C13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>36</v>
       </c>
-      <c r="E13">
+      <c r="G13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" t="s">
         <v>39</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1369,16 +1482,19 @@
         <v>41</v>
       </c>
       <c r="C15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" t="s">
         <v>8</v>
       </c>
-      <c r="D15" t="s">
+      <c r="F15" t="s">
         <v>42</v>
       </c>
-      <c r="E15">
+      <c r="G15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -1386,16 +1502,19 @@
         <v>44</v>
       </c>
       <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" t="s">
         <v>8</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
         <v>42</v>
       </c>
-      <c r="E16">
+      <c r="G16">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1403,16 +1522,19 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" t="s">
         <v>8</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F17" t="s">
         <v>42</v>
       </c>
-      <c r="E17">
+      <c r="G17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1420,16 +1542,19 @@
         <v>48</v>
       </c>
       <c r="C18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" t="s">
         <v>8</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" t="s">
         <v>42</v>
       </c>
-      <c r="E18">
+      <c r="G18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -1437,50 +1562,53 @@
         <v>50</v>
       </c>
       <c r="C19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
         <v>51</v>
       </c>
-      <c r="E19">
+      <c r="G19">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
       <c r="B20" t="s">
         <v>53</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>8</v>
       </c>
-      <c r="D20" t="s">
+      <c r="F20" t="s">
         <v>54</v>
       </c>
-      <c r="E20">
+      <c r="G20">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>55</v>
       </c>
       <c r="B21" t="s">
         <v>56</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>8</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
         <v>57</v>
       </c>
-      <c r="E21">
+      <c r="G21">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -1488,16 +1616,19 @@
         <v>59</v>
       </c>
       <c r="C22" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" t="s">
         <v>60</v>
       </c>
-      <c r="D22" t="s">
+      <c r="F22" t="s">
         <v>61</v>
       </c>
-      <c r="E22">
+      <c r="G22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -1505,16 +1636,19 @@
         <v>63</v>
       </c>
       <c r="C23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" t="s">
         <v>64</v>
       </c>
-      <c r="D23" t="s">
+      <c r="F23" t="s">
         <v>65</v>
       </c>
-      <c r="E23">
+      <c r="G23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -1522,16 +1656,19 @@
         <v>67</v>
       </c>
       <c r="C24" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" t="s">
         <v>68</v>
       </c>
-      <c r="D24" t="s">
+      <c r="F24" t="s">
         <v>69</v>
       </c>
-      <c r="E24">
+      <c r="G24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>70</v>
       </c>
@@ -1539,16 +1676,19 @@
         <v>71</v>
       </c>
       <c r="C25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" t="s">
         <v>72</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" t="s">
         <v>73</v>
       </c>
-      <c r="E25">
+      <c r="G25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -1556,12 +1696,15 @@
         <v>75</v>
       </c>
       <c r="C26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" t="s">
         <v>76</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>77</v>
       </c>
-      <c r="E26">
+      <c r="G26">
         <v>4</v>
       </c>
     </row>

</xml_diff>